<commit_message>
Univariate Gaussian Classifier Example Added
</commit_message>
<xml_diff>
--- a/ML_Unit4/excel/numeric_examples.xlsx
+++ b/ML_Unit4/excel/numeric_examples.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93c4ddfd9869a0cf/consulting/dono/idma_pt_public/ML_Unit4/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="8_{F1D6EBA1-8E1B-194D-96A4-BAC16A1FB37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27A1F68C-269D-9E40-870E-4BD0D5B9C36F}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="8_{F1D6EBA1-8E1B-194D-96A4-BAC16A1FB37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07395C55-9899-F64F-9AF8-76C4D257C13D}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" xr2:uid="{9B9E1C1F-324F-B14F-9EF7-2314F08EEAD2}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15700" activeTab="1" xr2:uid="{9B9E1C1F-324F-B14F-9EF7-2314F08EEAD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Multinomial  Model" sheetId="1" r:id="rId1"/>
+    <sheet name="Univariate Gaussian" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Docs</t>
   </si>
@@ -115,6 +116,45 @@
   </si>
   <si>
     <t>Size of Vocab</t>
+  </si>
+  <si>
+    <t>How python networking works</t>
+  </si>
+  <si>
+    <t>Blood Sugar</t>
+  </si>
+  <si>
+    <t>Diabetic</t>
+  </si>
+  <si>
+    <t>Mean Diabetic 0</t>
+  </si>
+  <si>
+    <t>Mean Diabetic 1</t>
+  </si>
+  <si>
+    <t>Variance Diabetic 0</t>
+  </si>
+  <si>
+    <t>Variance Diabetic 1</t>
+  </si>
+  <si>
+    <t>Training Data</t>
+  </si>
+  <si>
+    <t>Inference</t>
+  </si>
+  <si>
+    <t>Likelihood P(X|C=0)</t>
+  </si>
+  <si>
+    <t>Likelihood P(X|C=1)</t>
+  </si>
+  <si>
+    <t>Decision Rule</t>
+  </si>
+  <si>
+    <t>P(X|C=0)/P(X|C=1)</t>
   </si>
 </sst>
 </file>
@@ -195,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -209,6 +249,18 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389B9192-34D0-7E49-B4FE-DC7951E6D990}">
   <dimension ref="B1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A5" zoomScale="178" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -664,7 +716,10 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B8" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
@@ -831,4 +886,245 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94940190-EB6A-364B-AD05-2CEF02172E65}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="12">
+        <v>10</v>
+      </c>
+      <c r="B3" s="12">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <f>AVERAGE(A3:A8)</f>
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <f>AVERAGE(A9:A14)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
+        <v>8</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="12">
+        <v>10</v>
+      </c>
+      <c r="B5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
+        <v>10</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <f>STDEVP(A3:A8)^2</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <f>STDEVP(A9:A14)^2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="12">
+        <v>11</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
+        <v>11</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="12">
+        <v>12</v>
+      </c>
+      <c r="B9" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="12">
+        <v>15</v>
+      </c>
+      <c r="B11" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="12">
+        <v>13</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="1">
+        <f>_xlfn.NORM.DIST(A18,D$3,SQRT(D$6),FALSE)</f>
+        <v>0.3989422804014327</v>
+      </c>
+      <c r="E18" s="1">
+        <f>_xlfn.NORM.DIST(A18,E$3,SQRT(E$6),FALSE)</f>
+        <v>0.12098536225957168</v>
+      </c>
+      <c r="F18" s="1">
+        <f>D18/E18</f>
+        <v>3.2974425414002564</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="13">
+        <v>11</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="D19" s="1">
+        <f>_xlfn.NORM.DIST(A19,D$3,SQRT(D$6),FALSE)</f>
+        <v>0.24197072451914337</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" ref="E19:E20" si="0">_xlfn.NORM.DIST(A19,E$3,SQRT(E$6),FALSE)</f>
+        <v>0.17603266338214976</v>
+      </c>
+      <c r="F19" s="1">
+        <f>D19/E19</f>
+        <v>1.3745785575819442</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="D20" s="1">
+        <f>_xlfn.NORM.DIST(A20,D$3,SQRT(D$6),FALSE)</f>
+        <v>1.3383022576488537E-4</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2159242059690038E-3</v>
+      </c>
+      <c r="F20" s="1">
+        <f>D20/E20</f>
+        <v>6.0394766844637002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added lecture 16 deck, expectation maximization.pptx
</commit_message>
<xml_diff>
--- a/ML_Unit4/excel/numeric_examples.xlsx
+++ b/ML_Unit4/excel/numeric_examples.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93c4ddfd9869a0cf/consulting/dono/idma_pt_public/ML_Unit4/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="8_{F1D6EBA1-8E1B-194D-96A4-BAC16A1FB37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07395C55-9899-F64F-9AF8-76C4D257C13D}"/>
+  <xr:revisionPtr revIDLastSave="400" documentId="8_{F1D6EBA1-8E1B-194D-96A4-BAC16A1FB37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A62B37A7-BB92-8C4A-93EB-A4F952CE67DA}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15700" activeTab="1" xr2:uid="{9B9E1C1F-324F-B14F-9EF7-2314F08EEAD2}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15700" activeTab="2" xr2:uid="{9B9E1C1F-324F-B14F-9EF7-2314F08EEAD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Multinomial  Model" sheetId="1" r:id="rId1"/>
     <sheet name="Univariate Gaussian" sheetId="2" r:id="rId2"/>
+    <sheet name="EM Example" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
   <si>
     <t>Docs</t>
   </si>
@@ -155,13 +156,88 @@
   </si>
   <si>
     <t>P(X|C=0)/P(X|C=1)</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x0</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>x4</t>
+  </si>
+  <si>
+    <t># clusters</t>
+  </si>
+  <si>
+    <t>Iteration 1</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>mu1</t>
+  </si>
+  <si>
+    <t>mu2</t>
+  </si>
+  <si>
+    <t>sigma1</t>
+  </si>
+  <si>
+    <t>sigma2</t>
+  </si>
+  <si>
+    <t>(Randomly Chosen)</t>
+  </si>
+  <si>
+    <t>E Step</t>
+  </si>
+  <si>
+    <t>pjN(xi,muj,sigmaj)</t>
+  </si>
+  <si>
+    <t>Point</t>
+  </si>
+  <si>
+    <t>P(1|i)</t>
+  </si>
+  <si>
+    <t>P(2|i)</t>
+  </si>
+  <si>
+    <t>M Step</t>
+  </si>
+  <si>
+    <t>n1</t>
+  </si>
+  <si>
+    <t>n2</t>
+  </si>
+  <si>
+    <t>log likelihood calculation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -177,6 +253,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,7 +276,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -231,11 +321,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -261,6 +362,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -892,7 +999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94940190-EB6A-364B-AD05-2CEF02172E65}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="125" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -1127,4 +1234,548 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E56E03-476E-9A4A-966B-C551C4F187A0}">
+  <dimension ref="A1:G45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="E2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="1">
+        <f>($B$9*_xlfn.NORM.DIST(B2,$B$11,$B$13,FALSE))</f>
+        <v>2.6766045152977075E-5</v>
+      </c>
+      <c r="C18" s="1">
+        <f>B18/(B18+F18)</f>
+        <v>2.9312230751356326E-2</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="1">
+        <f>($B$10*_xlfn.NORM.DIST(B2,$B$12,$B$14,FALSE))</f>
+        <v>8.8636968238760142E-4</v>
+      </c>
+      <c r="G18" s="1">
+        <f>F18/(F18+B18)</f>
+        <v>0.97068776924864364</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1">
+        <f>$B$9*_xlfn.NORM.DIST(B3,$B$11,$B$13,FALSE)</f>
+        <v>1.7453653900915205E-4</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" ref="C19:C22" si="0">B19/(B19+F19)</f>
+        <v>7.1131001663238685E-2</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" ref="F19:F22" si="1">($B$10*_xlfn.NORM.DIST(B3,$B$12,$B$14,FALSE))</f>
+        <v>2.2791972047594886E-3</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" ref="G19:G22" si="2">F19/(F19+B19)</f>
+        <v>0.9288689983367614</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="1">
+        <f>$B$9*_xlfn.NORM.DIST(B4,$B$11,$B$13,FALSE)</f>
+        <v>3.5056600987137081E-3</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.24508501313237172</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0798193302637612E-2</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="2"/>
+        <v>0.75491498686762826</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1">
+        <f>$B$9*_xlfn.NORM.DIST(B5,$B$11,$B$13,FALSE)</f>
+        <v>2.590351913317835E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.44124492765890372</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>3.2802014935198721E-2</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="2"/>
+        <v>0.55875507234109623</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="1">
+        <f>$B$9*_xlfn.NORM.DIST(B6,$B$11,$B$13,FALSE)</f>
+        <v>4.8394144903828679E-2</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8394144903828679E-2</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="17"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="15">
+        <f>SUM(C18:C22)</f>
+        <v>1.2867731732058705</v>
+      </c>
+      <c r="E23" s="15"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="17">
+        <f>SUM(G18:G22)</f>
+        <v>3.7132268267941297</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27">
+        <f>C23</f>
+        <v>1.2867731732058705</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28">
+        <f>G23</f>
+        <v>3.7132268267941297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29">
+        <f>B27/5</f>
+        <v>0.25735463464117408</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30">
+        <f>B28/5</f>
+        <v>0.74264536535882597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31">
+        <f>1/B27*(SUMPRODUCT(C18:C22,B2:B6))</f>
+        <v>3.6726266948626516</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32">
+        <f>1/B28*(SUMPRODUCT(G18:G22,B2:B6))</f>
+        <v>1.4203717520818746</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33">
+        <f>1/B27*(SQRT((B2-B31)^2+(B3-B31)^2+(B4-B31)^2+(B5-B31)^2+(B6-B31)^2))</f>
+        <v>4.9143379337243438</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34">
+        <f>1/B28*(SQRT((B2-B32)^2+(B3-B32)^2+(B4-B32)^2+(B5-B32)^2+(B6-B32)^2))</f>
+        <v>1.4168711057167118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37">
+        <f>LOG(B40+F40)+LOG(B41+F41)+LOG(B42+F42)+LOG(B43+F43)+LOG(B44+F44)</f>
+        <v>-1.9920492758953352</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="1">
+        <f>($B$27*_xlfn.NORM.DIST(B2,$B$31,$B$33,FALSE))</f>
+        <v>6.6471461118426681E-2</v>
+      </c>
+      <c r="C40" s="1">
+        <f>B40/(B40+F40)</f>
+        <v>0.21476590675370383</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="1">
+        <f>($B$28*_xlfn.NORM.DIST(B2,$B$32,$B$34,FALSE))</f>
+        <v>0.24303511803641548</v>
+      </c>
+      <c r="G40" s="1">
+        <f>F40/(F40+B40)</f>
+        <v>0.78523409324629623</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" ref="B41:B44" si="3">($B$27*_xlfn.NORM.DIST(B3,$B$31,$B$33,FALSE))</f>
+        <v>7.9007844168145769E-2</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" ref="C41:C44" si="4">B41/(B41+F41)</f>
+        <v>0.11103167003173831</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" ref="F41:F44" si="5">($B$28*_xlfn.NORM.DIST(B3,$B$32,$B$34,FALSE))</f>
+        <v>0.63257151103349574</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" ref="G41:G44" si="6">F41/(F41+B41)</f>
+        <v>0.88896832996826169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="3"/>
+        <v>9.858076000419641E-2</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="4"/>
+        <v>9.2985618788783433E-2</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="5"/>
+        <v>0.96159135357954306</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="6"/>
+        <v>0.90701438121121658</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="1">
+        <f t="shared" si="3"/>
+        <v>0.10422776268480052</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="4"/>
+        <v>0.34337208317027701</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="5"/>
+        <v>0.1993139863196296</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="6"/>
+        <v>0.6566279168297231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="1">
+        <f t="shared" si="3"/>
+        <v>0.1007175217150242</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="4"/>
+        <v>0.70087785828690063</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="5"/>
+        <v>4.2984437940542505E-2</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="6"/>
+        <v>0.29912214171309931</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="17"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="15">
+        <f>SUM(C40:C44)</f>
+        <v>1.4630331370314031</v>
+      </c>
+      <c r="E45" s="15"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="17">
+        <f>SUM(G40:G44)</f>
+        <v>3.5369668629685966</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>